<commit_message>
complete c and ghg diagnostics for all, region, and land type
</commit_message>
<xml_diff>
--- a/raw_data/scenario_headers.xlsx
+++ b/raw_data/scenario_headers.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26120" yWindow="0" windowWidth="22560" windowHeight="28340" tabRatio="500" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="26120" yWindow="0" windowWidth="22560" windowHeight="28340" tabRatio="500" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="area_2010" sheetId="12" r:id="rId1"/>
@@ -127,9 +127,6 @@
     <t># Annual target area of specific management within land types (or annual amount of area change for a land type), by land type and ownership class</t>
   </si>
   <si>
-    <t># Developed growth in 2010 matches the historical change datain annual_net_area_change; Developed urban forest is the % of developed_all for that year, in 2010 this is 14.4% of Developed_all with a 1995- 2016 trend of 0.1619% increase per year (based on recent work by John Dingman at ARB), also Dead_removal = Developed_all in any given year and must be caluculated from the initial area and growth rates (see Growth below)</t>
-  </si>
-  <si>
     <t># private non-cut treatments are a combination of state CFIP and WMP projects from the calfire vtp eir 2016 (14142.97 ha; 5.3-1, 2004-2013; targets add to this portion only), and federal projects (13784.66 ha, doesn't change; total annual average of 27927.63 ha reported by Jason Ko 2008-2015)</t>
   </si>
   <si>
@@ -152,6 +149,9 @@
   </si>
   <si>
     <t># water, ice, barren, sparse, desert,grassland, meadow, marshes, cultivated, and seagrass are assumed to have no mortality fraction because they do not have veg c accumulation in the carbon input file (mortality and transfer to soil is implicit in the soil c accumulation representing net c exchange)</t>
+  </si>
+  <si>
+    <t># Developed growth in 2010 matches the historical change datain annual_net_area_change; Developed urban forest is the fraction of developed_all for that year, in 2010 this is 14.4% of Developed_all with a 1995- 2016 trend of 0.1619% increase per year (based on recent work by John Dingman at ARB), also Dead_removal = Developed_all in any given year and must be caluculated from the initial area and growth rates (see Growth below)</t>
   </si>
 </sst>
 </file>
@@ -5078,8 +5078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5114,32 +5114,32 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="4" t="s">
+    <row r="8" spans="1:12">
+      <c r="A8" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="4" t="s">
+    <row r="9" spans="1:12">
+      <c r="A9" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
     <row r="10" spans="1:12">
       <c r="A10" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -6129,7 +6129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
@@ -6154,7 +6154,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -6179,12 +6179,12 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:8">

</xml_diff>

<commit_message>
changed all instances of Fuel_reduction to Thinning
</commit_message>
<xml_diff>
--- a/raw_data/scenario_headers.xlsx
+++ b/raw_data/scenario_headers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="72780" yWindow="2720" windowWidth="26260" windowHeight="13260" tabRatio="500" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15580" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="area_2010" sheetId="12" r:id="rId1"/>
@@ -108,9 +108,6 @@
     <t># private non-cut treatments are a combination of state CFIP and WMP projects from the calfire vtp eir 2016 (14142.97 ha; 5.3-1, 2004-2013; targets add to this portion only), and federal projects (13784.66 ha, doesn't change; total annual average of 27927.63 ha reported by Jason Ko 2008-2015)</t>
   </si>
   <si>
-    <t># private total fuel reduction area is split among fuel_reductions (30%), understory_treatment (20%), and prescribed_burn (50%) based on the calfire vtp eir 2016 (2-38) for the state projects; the federal projects all go to fuel_reduction and are constant across scenarios</t>
-  </si>
-  <si>
     <t># USFS area, and private fuel reduction thinning area, from 2008-2015 averages, from Jason Ko; 2000-2015 avg annual prescribed burn area from the FRAP fire perimeter data has been subtracted from the USFS fuel reduction thinning because it is a fuel reduction activity</t>
   </si>
   <si>
@@ -169,6 +166,9 @@
   </si>
   <si>
     <t># Units: Hectares; no NA values allowed</t>
+  </si>
+  <si>
+    <t># private total Thinning area is split among Thinnings (30%), understory_treatment (20%), and prescribed_burn (50%) based on the calfire vtp eir 2016 (2-38) for the state projects; the federal projects all go to Thinning and are constant across scenarios</t>
   </si>
 </sst>
 </file>
@@ -2453,7 +2453,7 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2919,7 +2919,7 @@
   <dimension ref="A1:AP80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:F59"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5104,7 +5104,7 @@
   <dimension ref="A1:N113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5124,7 +5124,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -5139,12 +5139,12 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -5154,17 +5154,17 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="4" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -5818,7 +5818,7 @@
   <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A3:A10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5844,27 +5844,27 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5879,7 +5879,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -6155,7 +6155,7 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6179,7 +6179,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -6204,17 +6204,17 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -6754,14 +6754,14 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -6771,12 +6771,12 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -6825,14 +6825,14 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -6842,12 +6842,12 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:1">

</xml_diff>

<commit_message>
New NWL scenario file includes Historical, BAU_NWL, and Ambitious. This required changing write_caland_inputs so that it can deal with overlapping practices in time, at least for the area-based ones. The fraction ones still need to be distinct in time. This is working but still need to look at outputs.
</commit_message>
<xml_diff>
--- a/raw_data/scenario_headers.xlsx
+++ b/raw_data/scenario_headers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15580" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="46940" windowHeight="19200" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="area_2010" sheetId="12" r:id="rId1"/>
@@ -105,13 +105,7 @@
     <t># Annual target area of specific management within land types (or annual amount of area change for a land type), by land type and ownership class</t>
   </si>
   <si>
-    <t># private non-cut treatments are a combination of state CFIP and WMP projects from the calfire vtp eir 2016 (14142.97 ha; 5.3-1, 2004-2013; targets add to this portion only), and federal projects (13784.66 ha, doesn't change; total annual average of 27927.63 ha reported by Jason Ko 2008-2015)</t>
-  </si>
-  <si>
     <t># USFS area, and private fuel reduction thinning area, from 2008-2015 averages, from Jason Ko; 2000-2015 avg annual prescribed burn area from the FRAP fire perimeter data has been subtracted from the USFS fuel reduction thinning because it is a fuel reduction activity</t>
-  </si>
-  <si>
-    <t># Private clearcut and partial cut area data from Robards and Nickerson 2013; grouped based on the treatments to match stewart and nakamura 2012</t>
   </si>
   <si>
     <t># fresh marsh baseline to 2020 is ecorestore target (1416.40 ha) is split between private and state_gov proportinoally to 2010 area of cultivated land (the source)in the Delta region</t>
@@ -168,7 +162,13 @@
     <t># Units: Hectares; no NA values allowed</t>
   </si>
   <si>
-    <t># private total Thinning area is split among Thinnings (30%), understory_treatment (20%), and prescribed_burn (50%) based on the calfire vtp eir 2016 (2-38) for the state projects; the federal projects all go to Thinning and are constant across scenarios</t>
+    <t># private total fuel reduction area is split among Thinnings (30%), understory_treatment (20%), and prescribed_burn (50%) based on the calfire vtp eir 2016 (2-38) for the state projects; the federal projects all go to Thinning and are constant across scenarios</t>
+  </si>
+  <si>
+    <t># Private clearcut and partial cut area data from Robards and Nickerson 2013; grouped based on the treatments to match stewart and nakamura 2012; regionalized based on 2010 CALAND private forest area</t>
+  </si>
+  <si>
+    <t># private non-clearcut and non-partial-cut treatments are a combination of state CFIP and WMP projects from the calfire vtp eir 2016 (14142.97 ha; 5.3-1, 2004-2013; targets add to this portion only), and federal projects (13784.66 ha, doesn't change; total annual average of 27927.63 ha reported by Jason Ko 2008-2015)</t>
   </si>
 </sst>
 </file>
@@ -5104,7 +5104,7 @@
   <dimension ref="A1:N113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5124,7 +5124,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -5139,32 +5139,32 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="4" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="4" t="s">
-        <v>28</v>
+      <c r="A10" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -5844,27 +5844,27 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5879,7 +5879,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -6179,7 +6179,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -6204,17 +6204,17 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -6761,7 +6761,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -6771,12 +6771,12 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -6832,7 +6832,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -6842,12 +6842,12 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:1">

</xml_diff>

<commit_message>
Updated plot_scen_types.r to deal with ownership specific outputs, and plot legends have shorter names; added v4 and v5 scenario files; removed scenarios prior to v4; plot_caland.r legend labels are still the full scenario file name because of all the distinctions - need to figure out how to deal with this
</commit_message>
<xml_diff>
--- a/raw_data/scenario_headers.xlsx
+++ b/raw_data/scenario_headers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="46940" windowHeight="19200" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="59720" yWindow="6680" windowWidth="32000" windowHeight="21600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="area_2010" sheetId="12" r:id="rId1"/>
@@ -123,9 +123,6 @@
     <t># developed_all mortality is transferred to harvest because it is highly managed; this allows for more control over the emissions pathway of this mortality</t>
   </si>
   <si>
-    <t># Developed growth in 2010 matches the historical change datain annual_net_area_change; Developed urban forest is the fraction of developed_all for that year, in 2010 this is 14.4% of Developed_all with a 1995- 2016 trend of 0.1619% increase per year (based on recent work by John Dingman at ARB), also Dead_removal = Developed_all area in any given year and must be caluculated from the initial area and growth rates (see Growth below)</t>
-  </si>
-  <si>
     <t># These data are from the CA fourth assessment</t>
   </si>
   <si>
@@ -169,6 +166,9 @@
   </si>
   <si>
     <t># private non-clearcut and non-partial-cut treatments are a combination of state CFIP and WMP projects from the calfire vtp eir 2016 (14142.97 ha; 5.3-1, 2004-2013; targets add to this portion only), and federal projects (13784.66 ha, doesn't change; total annual average of 27927.63 ha reported by Jason Ko 2008-2015)</t>
+  </si>
+  <si>
+    <t># Developed growth in 2010 matches the historical change data; Developed urban forest is the % of developed all for that year, in 2010 this is 15% of Developed_all (this is the historical baseline) annual increases are prescribed in target scenarios; Dead_removal is applied to the total developed_all area because that is the area basis for the urban forest values</t>
   </si>
 </sst>
 </file>
@@ -5104,7 +5104,7 @@
   <dimension ref="A1:N113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5124,7 +5124,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -5139,7 +5139,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -5149,12 +5149,12 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -5164,7 +5164,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -5844,27 +5844,27 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5879,7 +5879,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -6761,7 +6761,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -6771,12 +6771,12 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -6832,7 +6832,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -6842,12 +6842,12 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:1">

</xml_diff>